<commit_message>
Treatments, Reagents, and Reagent Sets
</commit_message>
<xml_diff>
--- a/ImmPort/CompletedTemplates/reagents.Flow_Cytometry.xlsx
+++ b/ImmPort/CompletedTemplates/reagents.Flow_Cytometry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drach\Documents\AlphaBeta\ImmPort\CompletedTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F55FC3-059D-4304-BAFE-B235AA5F673F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A264C6A3-13E9-4AD6-9752-CE065FDFDCA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -202,7 +202,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1105" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="1046">
   <si>
     <t>flow_cytometry_reagents</t>
   </si>
@@ -3328,6 +3328,18 @@
   </si>
   <si>
     <t>Alexa Fluor 488 CD3</t>
+  </si>
+  <si>
+    <t>Alexa Fluor 488 hCD1d unloaded</t>
+  </si>
+  <si>
+    <t>hCD1d unloaded</t>
+  </si>
+  <si>
+    <t>Alexa Fluor 647 hMR1 6-FP</t>
+  </si>
+  <si>
+    <t>hMR1 6-FP</t>
   </si>
 </sst>
 </file>
@@ -3780,10 +3792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M200"/>
+  <dimension ref="A1:M202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4247,187 +4259,187 @@
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" t="s">
-        <v>997</v>
+        <v>1042</v>
       </c>
       <c r="E23" t="s">
-        <v>961</v>
-      </c>
-      <c r="F23">
-        <v>342906</v>
+        <v>994</v>
+      </c>
+      <c r="F23" t="s">
+        <v>1040</v>
       </c>
       <c r="J23" t="s">
-        <v>998</v>
+        <v>1043</v>
       </c>
       <c r="L23" t="s">
-        <v>999</v>
+        <v>1040</v>
       </c>
       <c r="M23" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="3"/>
       <c r="B24" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="E24" t="s">
         <v>961</v>
       </c>
       <c r="F24">
-        <v>320806</v>
+        <v>342906</v>
       </c>
       <c r="J24" t="s">
-        <v>301</v>
+        <v>998</v>
       </c>
       <c r="L24" t="s">
-        <v>1002</v>
+        <v>999</v>
       </c>
       <c r="M24" t="s">
-        <v>1003</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" t="s">
-        <v>1004</v>
+        <v>1001</v>
       </c>
       <c r="E25" t="s">
         <v>961</v>
       </c>
       <c r="F25">
-        <v>302716</v>
+        <v>320806</v>
       </c>
       <c r="J25" t="s">
-        <v>245</v>
+        <v>301</v>
       </c>
       <c r="L25" t="s">
-        <v>1005</v>
+        <v>1002</v>
       </c>
       <c r="M25" t="s">
-        <v>1006</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" t="s">
-        <v>1007</v>
+        <v>1004</v>
       </c>
       <c r="E26" t="s">
-        <v>938</v>
+        <v>961</v>
       </c>
       <c r="F26">
-        <v>555433</v>
+        <v>302716</v>
       </c>
       <c r="J26" t="s">
-        <v>1008</v>
+        <v>245</v>
       </c>
       <c r="L26" t="s">
-        <v>1009</v>
+        <v>1005</v>
       </c>
       <c r="M26" t="s">
-        <v>1010</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="3"/>
       <c r="B27" t="s">
-        <v>1011</v>
+        <v>1007</v>
       </c>
       <c r="E27" t="s">
-        <v>961</v>
+        <v>938</v>
       </c>
       <c r="F27">
-        <v>502946</v>
+        <v>555433</v>
       </c>
       <c r="J27" t="s">
-        <v>877</v>
+        <v>1008</v>
       </c>
       <c r="L27" t="s">
-        <v>1012</v>
+        <v>1009</v>
       </c>
       <c r="M27" t="s">
-        <v>1013</v>
+        <v>1010</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="3"/>
       <c r="B28" t="s">
-        <v>1014</v>
+        <v>1011</v>
       </c>
       <c r="E28" t="s">
-        <v>1015</v>
-      </c>
-      <c r="F28" t="s">
-        <v>1016</v>
+        <v>961</v>
+      </c>
+      <c r="F28">
+        <v>502946</v>
       </c>
       <c r="J28" t="s">
-        <v>821</v>
+        <v>877</v>
       </c>
       <c r="L28" t="s">
-        <v>1017</v>
+        <v>1012</v>
       </c>
       <c r="M28" t="s">
-        <v>1018</v>
+        <v>1013</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
       <c r="B29" t="s">
-        <v>1019</v>
+        <v>1014</v>
       </c>
       <c r="E29" t="s">
-        <v>961</v>
-      </c>
-      <c r="F29">
-        <v>302012</v>
+        <v>1015</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1016</v>
       </c>
       <c r="J29" t="s">
-        <v>146</v>
+        <v>821</v>
       </c>
       <c r="L29" t="s">
-        <v>1020</v>
+        <v>1017</v>
       </c>
       <c r="M29" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
       <c r="B30" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="E30" t="s">
-        <v>994</v>
-      </c>
-      <c r="F30" t="s">
-        <v>1040</v>
+        <v>961</v>
+      </c>
+      <c r="F30">
+        <v>302012</v>
       </c>
       <c r="J30" t="s">
-        <v>1023</v>
+        <v>146</v>
       </c>
       <c r="L30" t="s">
-        <v>1040</v>
+        <v>1020</v>
       </c>
       <c r="M30" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="3"/>
       <c r="B31" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="E31" t="s">
-        <v>961</v>
-      </c>
-      <c r="F31">
-        <v>351726</v>
+        <v>994</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1040</v>
       </c>
       <c r="J31" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="L31" t="s">
-        <v>1027</v>
+        <v>1040</v>
       </c>
       <c r="M31" t="s">
         <v>1024</v>
@@ -4436,137 +4448,149 @@
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="3"/>
       <c r="B32" t="s">
-        <v>1028</v>
+        <v>1044</v>
       </c>
       <c r="E32" t="s">
-        <v>938</v>
-      </c>
-      <c r="F32">
-        <v>565184</v>
+        <v>994</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1040</v>
       </c>
       <c r="J32" t="s">
-        <v>98</v>
+        <v>1045</v>
       </c>
       <c r="L32" t="s">
-        <v>1029</v>
+        <v>1040</v>
       </c>
       <c r="M32" t="s">
-        <v>1030</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="3"/>
       <c r="B33" t="s">
-        <v>1031</v>
+        <v>1025</v>
       </c>
       <c r="E33" t="s">
         <v>961</v>
       </c>
       <c r="F33">
-        <v>302846</v>
+        <v>351726</v>
       </c>
       <c r="J33" t="s">
-        <v>248</v>
+        <v>1026</v>
       </c>
       <c r="L33" t="s">
-        <v>1032</v>
+        <v>1027</v>
       </c>
       <c r="M33" t="s">
-        <v>1033</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
       <c r="B34" t="s">
-        <v>1034</v>
+        <v>1028</v>
       </c>
       <c r="E34" t="s">
-        <v>961</v>
+        <v>938</v>
       </c>
       <c r="F34">
-        <v>303550</v>
+        <v>565184</v>
       </c>
       <c r="J34" t="s">
-        <v>335</v>
+        <v>98</v>
       </c>
       <c r="L34" t="s">
-        <v>1035</v>
+        <v>1029</v>
       </c>
       <c r="M34" t="s">
-        <v>1036</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="3"/>
       <c r="B35" t="s">
-        <v>1041</v>
+        <v>1031</v>
       </c>
       <c r="E35" t="s">
         <v>961</v>
       </c>
       <c r="F35">
-        <v>300415</v>
+        <v>302846</v>
       </c>
       <c r="J35" t="s">
-        <v>279</v>
+        <v>248</v>
       </c>
       <c r="L35" t="s">
-        <v>1038</v>
+        <v>1032</v>
       </c>
       <c r="M35" t="s">
-        <v>996</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="3"/>
       <c r="B36" t="s">
-        <v>1037</v>
+        <v>1034</v>
       </c>
       <c r="E36" t="s">
         <v>961</v>
       </c>
       <c r="F36">
-        <v>317312</v>
+        <v>303550</v>
       </c>
       <c r="J36" t="s">
-        <v>279</v>
+        <v>335</v>
       </c>
       <c r="L36" t="s">
-        <v>1039</v>
+        <v>1035</v>
       </c>
       <c r="M36" t="s">
-        <v>1024</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="3"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="3"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
+      <c r="B37" t="s">
+        <v>1041</v>
+      </c>
+      <c r="E37" t="s">
+        <v>961</v>
+      </c>
+      <c r="F37">
+        <v>300415</v>
+      </c>
+      <c r="J37" t="s">
+        <v>279</v>
+      </c>
+      <c r="L37" t="s">
+        <v>1038</v>
+      </c>
+      <c r="M37" t="s">
+        <v>996</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="3"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="1"/>
-      <c r="M38" s="1"/>
+      <c r="B38" t="s">
+        <v>1037</v>
+      </c>
+      <c r="E38" t="s">
+        <v>961</v>
+      </c>
+      <c r="F38">
+        <v>317312</v>
+      </c>
+      <c r="J38" t="s">
+        <v>279</v>
+      </c>
+      <c r="L38" t="s">
+        <v>1039</v>
+      </c>
+      <c r="M38" t="s">
+        <v>1024</v>
+      </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="3"/>
@@ -6998,9 +7022,39 @@
       <c r="L200" s="1"/>
       <c r="M200" s="1"/>
     </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A201" s="3"/>
+      <c r="B201" s="1"/>
+      <c r="C201" s="3"/>
+      <c r="D201" s="3"/>
+      <c r="E201" s="1"/>
+      <c r="F201" s="1"/>
+      <c r="G201" s="3"/>
+      <c r="H201" s="3"/>
+      <c r="I201" s="3"/>
+      <c r="J201" s="1"/>
+      <c r="K201" s="3"/>
+      <c r="L201" s="1"/>
+      <c r="M201" s="1"/>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A202" s="3"/>
+      <c r="B202" s="1"/>
+      <c r="C202" s="3"/>
+      <c r="D202" s="3"/>
+      <c r="E202" s="1"/>
+      <c r="F202" s="1"/>
+      <c r="G202" s="3"/>
+      <c r="H202" s="3"/>
+      <c r="I202" s="3"/>
+      <c r="J202" s="1"/>
+      <c r="K202" s="3"/>
+      <c r="L202" s="1"/>
+      <c r="M202" s="1"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Analyte Reported" error="Preferred value was not selected" promptTitle="Analyte Reported" prompt="Please choose preferred value from the list" sqref="J4:J201" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" errorTitle="Analyte Reported" error="Preferred value was not selected" promptTitle="Analyte Reported" prompt="Please choose preferred value from the list" sqref="J4:J203" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>lookupanalyte_reported1147</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>